<commit_message>
tab names has spaces
</commit_message>
<xml_diff>
--- a/Salaries.xlsx
+++ b/Salaries.xlsx
@@ -13,12 +13,12 @@
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId3"/>
-    <sheet name="emp1" sheetId="7" r:id="rId4"/>
-    <sheet name="emp2" sheetId="4" r:id="rId5"/>
-    <sheet name="emp3" sheetId="5" r:id="rId6"/>
-    <sheet name="emp4" sheetId="6" r:id="rId7"/>
+    <sheet name="f1 l1" sheetId="8" r:id="rId2"/>
+    <sheet name="f2 l2" sheetId="9" r:id="rId3"/>
+    <sheet name="sairandhree sule" sheetId="7" r:id="rId4"/>
+    <sheet name="ajay wani" sheetId="4" r:id="rId5"/>
+    <sheet name="akshay patil" sheetId="5" r:id="rId6"/>
+    <sheet name="pooja joshi" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" calcMode="manual"/>
   <customWorkbookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>emp3</t>
   </si>
   <si>
-    <t>emp5</t>
-  </si>
-  <si>
     <t>B222</t>
   </si>
   <si>
@@ -82,6 +79,21 @@
   </si>
   <si>
     <t>sd</t>
+  </si>
+  <si>
+    <t>sairandhree sule</t>
+  </si>
+  <si>
+    <t>Ajay Wani</t>
+  </si>
+  <si>
+    <t>Akshay Patil</t>
+  </si>
+  <si>
+    <t>Pooja Joshi</t>
+  </si>
+  <si>
+    <t>Temp emp</t>
   </si>
 </sst>
 </file>
@@ -918,7 +930,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -938,42 +950,42 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1001,7 +1013,7 @@
   <sheetData>
     <row r="12" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1021,12 +1033,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1068,7 +1080,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
configuration added to sendEmail
</commit_message>
<xml_diff>
--- a/Salaries.xlsx
+++ b/Salaries.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14060" windowHeight="6090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14063" windowHeight="6090"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -94,13 +94,37 @@
   </si>
   <si>
     <t>Temp emp</t>
+  </si>
+  <si>
+    <t>f1 l1</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>sairandhre.sule+ss@niyuj.com</t>
+  </si>
+  <si>
+    <t>sairandhre.sule+aw@niyuj.com</t>
+  </si>
+  <si>
+    <t>sairandhre.sule+ap@niyuj.com</t>
+  </si>
+  <si>
+    <t>sairandhre.sule+pj@niyuj.com</t>
+  </si>
+  <si>
+    <t>sairandhre.sule+te@niyuj.com</t>
+  </si>
+  <si>
+    <t>sairandhre.sule+fl@niyuj.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +256,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,7 +566,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -577,12 +609,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -616,6 +650,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -927,20 +962,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="16.796875" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="24.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -948,45 +983,86 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C13" s="2"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -996,8 +1072,16 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C7" r:id="rId5"/>
+    <hyperlink ref="C8" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1009,9 +1093,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1029,14 +1113,14 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -1055,9 +1139,9 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1065,7 +1149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1073,12 +1157,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1097,9 +1181,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1115,7 +1199,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1134,9 +1218,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1152,7 +1236,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1171,9 +1255,9 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1181,7 +1265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1189,7 +1273,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>

</xml_diff>